<commit_message>
default object field separator change from : to ;
</commit_message>
<xml_diff>
--- a/raw/zh/sample.xlsx
+++ b/raw/zh/sample.xlsx
@@ -1,191 +1,165 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView windowWidth="28125" windowHeight="12540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="英雄|Hero" sheetId="1" r:id="rId1"/>
     <sheet name="全局参数|Global" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="60">
+  <si>
+    <t>索引</t>
+  </si>
+  <si>
+    <t>名称</t>
+  </si>
+  <si>
+    <t>坐骑</t>
+  </si>
+  <si>
+    <t>性别</t>
+  </si>
+  <si>
+    <t>身高</t>
+  </si>
+  <si>
+    <t>武器</t>
+  </si>
+  <si>
+    <t>主要属性</t>
+  </si>
+  <si>
+    <t>背包</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>int(Mount.Id)</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>int[]</t>
+  </si>
+  <si>
+    <t>{int Hp;int Magic}</t>
+  </si>
+  <si>
+    <t>{int Id;int Count}[]</t>
+  </si>
   <si>
     <t>Id</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>索引</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>名称</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Name</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>性别</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>MountId</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Weapon</t>
+  </si>
+  <si>
+    <t>Property</t>
+  </si>
+  <si>
+    <t>Bag</t>
   </si>
   <si>
     <t>server/client</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>bool</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sex</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>client</t>
   </si>
   <si>
     <t>奥丁</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1001</t>
+  </si>
+  <si>
+    <t>20000;10000</t>
+  </si>
+  <si>
+    <t>10001;10,10002;100,10003;25</t>
   </si>
   <si>
     <t>托尔</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1002</t>
+  </si>
+  <si>
+    <t>30000;1000</t>
+  </si>
+  <si>
+    <t>10001;7,10002;101,10003;26</t>
   </si>
   <si>
     <t>希芙</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>武器</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>身高</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>double</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Height</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>int[]</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Weapon</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>1001</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>1002</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>1003,1004,1005</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>主要属性</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>{int Hp:int Magic}</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Property</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>20000:10000</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>30000:1000</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>10000:20000</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>背包</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>{int Id:int Count}[]</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bag</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>10001:10,10002:100,10003:25</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>10001:7,10002:101,10003:26</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>10004:35,10002:20,10003:100</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>10000;20000</t>
+  </si>
+  <si>
+    <t>10004;35,10002;20,10003;100</t>
   </si>
   <si>
     <t>name</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>value</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>type</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>sign</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>description</t>
   </si>
   <si>
     <t>NameLimit</t>
-    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>7</t>
-    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>i</t>
     </r>
     <r>
@@ -193,24 +167,27 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="等线"/>
-        <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>nt</t>
     </r>
-    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>client/server</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>名字字数限制</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>H</t>
     </r>
     <r>
@@ -218,20 +195,24 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="等线"/>
-        <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>itCorrection</t>
     </r>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>1</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>d</t>
     </r>
     <r>
@@ -239,143 +220,218 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="等线"/>
-        <family val="2"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>ouble</t>
     </r>
-    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>server</t>
   </si>
   <si>
     <t>命中修正系数</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>LevelRange</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>{int Min:int Max}</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>client/server</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1;99</t>
+  </si>
+  <si>
+    <t>{int Min;int Max}</t>
   </si>
   <si>
     <t>等级区间</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>1:99</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>InitItem</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>1001,1002,1003</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>int[]</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>server</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>server</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>初始任务获得道具</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>server/client</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>client</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>server/client</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>坐骑</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>server/client</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>MountId</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>int(Mount.Id)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
-      <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
-      <family val="2"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="等线"/>
-      <family val="2"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -384,12 +440,198 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="0" tint="-0.149998474074526"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -397,48 +639,334 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="50" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="13" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="51">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 5" xfId="1"/>
-    <cellStyle name="常规 6" xfId="2"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="常规 6" xfId="13"/>
+    <cellStyle name="注释" xfId="14" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="15" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="16" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="17" builtinId="11"/>
+    <cellStyle name="标题" xfId="18" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="19" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="20" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="21" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="22" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="23" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="24" builtinId="44"/>
+    <cellStyle name="输出" xfId="25" builtinId="21"/>
+    <cellStyle name="计算" xfId="26" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="27" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="28" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="30" builtinId="24"/>
+    <cellStyle name="汇总" xfId="31" builtinId="25"/>
+    <cellStyle name="好" xfId="32" builtinId="26"/>
+    <cellStyle name="适中" xfId="33" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="34" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="35" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="36" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="37" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="38" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="39" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="40" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="41" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="42" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="43" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="44" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="45" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="46" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="47" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="48" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="49" builtinId="52"/>
+    <cellStyle name="常规 5" xfId="50"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -452,7 +980,7 @@
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="16" name="直接箭头连接符 15"/>
         <xdr:cNvCxnSpPr/>
@@ -499,7 +1027,7 @@
       <xdr:row>36</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="17" name="文本框 16"/>
         <xdr:cNvSpPr txBox="1"/>
@@ -507,7 +1035,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2409825" y="5715000"/>
-          <a:ext cx="3943350" cy="828675"/>
+          <a:ext cx="10848975" cy="828675"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -600,14 +1128,14 @@
       <xdr:row>13</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="文本框 1"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="295276" y="2000250"/>
+          <a:off x="295275" y="2000250"/>
           <a:ext cx="4495800" cy="523875"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -662,6 +1190,7 @@
             <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
             <a:t>字段</a:t>
           </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -680,7 +1209,7 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
+    <xdr:cxnSp>
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="4" name="直接箭头连接符 3"/>
         <xdr:cNvCxnSpPr/>
@@ -760,7 +1289,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -793,26 +1322,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -845,23 +1357,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1003,146 +1498,141 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="6" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="15.125" customWidth="1"/>
     <col min="2" max="2" width="17.375" customWidth="1"/>
     <col min="3" max="3" width="18.5" customWidth="1"/>
     <col min="4" max="4" width="14.625" customWidth="1"/>
     <col min="5" max="5" width="22.875" customWidth="1"/>
-    <col min="6" max="6" width="25.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.25" customWidth="1"/>
+    <col min="6" max="6" width="25.5" style="2" customWidth="1"/>
+    <col min="7" max="7" width="29" customWidth="1"/>
     <col min="8" max="8" width="30.75" customWidth="1"/>
     <col min="9" max="9" width="14.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" s="1" customFormat="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" spans="1:8">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="4" t="s">
+      <c r="H2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="1" spans="1:8">
+      <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>28</v>
+      <c r="H3" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>29</v>
+    <row r="4" s="1" customFormat="1" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="C5">
         <v>10001</v>
@@ -1153,22 +1643,22 @@
       <c r="E5">
         <v>1.81</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>19</v>
+      <c r="F5" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="G5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="C6">
         <v>10002</v>
@@ -1179,22 +1669,22 @@
       <c r="E6">
         <v>1.86</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>20</v>
+      <c r="F6" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="G6" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="H6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="A7">
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1202,129 +1692,130 @@
       <c r="E7">
         <v>1.72</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>21</v>
+      <c r="F7" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="G7" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="H7" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="4" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="16.75" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.75" style="2" customWidth="1"/>
     <col min="3" max="3" width="19.375" customWidth="1"/>
     <col min="4" max="4" width="19.75" customWidth="1"/>
     <col min="5" max="5" width="33.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="4" t="s">
+    <row r="1" s="1" customFormat="1" spans="1:5">
+      <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="B1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" s="2" t="s">
+    <row r="2" spans="1:5">
+      <c r="A2" s="4" t="s">
         <v>43</v>
       </c>
+      <c r="B2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="2" t="s">
+    <row r="3" spans="1:5">
+      <c r="A3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="B5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D5" t="s">
-        <v>56</v>
-      </c>
       <c r="E5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>